<commit_message>
update seagrass field sheets
</commit_message>
<xml_diff>
--- a/seagrass/initial_datasheets/MarineGEO-Seagrass-Shoots_blade_measurements_v0.5.0.xlsx
+++ b/seagrass/initial_datasheets/MarineGEO-Seagrass-Shoots_blade_measurements_v0.5.0.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Dropbox (Smithsonian)\MarineGEO\Research\Modules\Seagrasses\seagrass-shoots\Fieldsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Repositories\protocols\seagrass\initial_datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BABAF7D-40C0-4C97-938A-846E0DBDE613}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD75094-8D0C-44AB-B389-B904CC154BB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="weighed_epifauna" sheetId="1" r:id="rId1"/>
+    <sheet name="shoots blade measures" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -590,77 +590,77 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1031,7 +1031,7 @@
   <dimension ref="A1:P54"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="112" zoomScaleNormal="100" zoomScalePageLayoutView="112" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:K5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
@@ -1056,24 +1056,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="20.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
     </row>
     <row r="2" spans="1:16" ht="16.5" customHeight="1">
       <c r="A2" s="3" t="s">
@@ -1090,90 +1090,90 @@
       <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:16" ht="31.5" customHeight="1">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="32" t="s">
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="36" t="s">
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="37"/>
-      <c r="K3" s="38"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="42"/>
       <c r="L3" s="13"/>
       <c r="M3" s="13"/>
       <c r="N3" s="13"/>
     </row>
     <row r="4" spans="1:16" ht="31.5" customHeight="1">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="32" t="s">
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="33"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="36" t="s">
+      <c r="J4" s="38"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="37"/>
-      <c r="N4" s="38"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="42"/>
     </row>
     <row r="5" spans="1:16" ht="32.25" customHeight="1">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="31" t="s">
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="41"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="45"/>
     </row>
     <row r="6" spans="1:16" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
     </row>
     <row r="7" spans="1:16" ht="34.5" customHeight="1">
       <c r="A7" s="11" t="s">
@@ -1182,18 +1182,18 @@
       <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="42" t="s">
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="43" t="s">
+      <c r="G7" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="44" t="s">
+      <c r="H7" s="25" t="s">
         <v>10</v>
       </c>
       <c r="I7" s="11" t="s">
@@ -1202,35 +1202,35 @@
       <c r="J7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="27" t="s">
+      <c r="K7" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="42" t="s">
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="O7" s="43" t="s">
+      <c r="O7" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="44" t="s">
+      <c r="P7" s="25" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="18" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" s="10"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
       <c r="F8" s="19"/>
       <c r="G8" s="8"/>
       <c r="H8" s="20"/>
       <c r="I8" s="8"/>
       <c r="J8" s="22"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
       <c r="N8" s="19"/>
       <c r="O8" s="8"/>
       <c r="P8" s="20"/>
@@ -1238,17 +1238,17 @@
     <row r="9" spans="1:16" ht="18" customHeight="1">
       <c r="A9" s="7"/>
       <c r="B9" s="9"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
       <c r="F9" s="14"/>
       <c r="G9" s="7"/>
       <c r="H9" s="15"/>
       <c r="I9" s="7"/>
       <c r="J9" s="21"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
       <c r="N9" s="14"/>
       <c r="O9" s="7"/>
       <c r="P9" s="15"/>
@@ -1256,17 +1256,17 @@
     <row r="10" spans="1:16" ht="18" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
       <c r="F10" s="19"/>
       <c r="G10" s="8"/>
       <c r="H10" s="20"/>
       <c r="I10" s="8"/>
       <c r="J10" s="22"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
       <c r="N10" s="19"/>
       <c r="O10" s="8"/>
       <c r="P10" s="20"/>
@@ -1274,17 +1274,17 @@
     <row r="11" spans="1:16" ht="18" customHeight="1">
       <c r="A11" s="7"/>
       <c r="B11" s="9"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
       <c r="F11" s="14"/>
       <c r="G11" s="7"/>
       <c r="H11" s="15"/>
       <c r="I11" s="7"/>
       <c r="J11" s="21"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
       <c r="N11" s="14"/>
       <c r="O11" s="7"/>
       <c r="P11" s="15"/>
@@ -1292,17 +1292,17 @@
     <row r="12" spans="1:16" ht="18" customHeight="1">
       <c r="A12" s="8"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="19"/>
       <c r="G12" s="8"/>
       <c r="H12" s="20"/>
       <c r="I12" s="8"/>
       <c r="J12" s="22"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
       <c r="N12" s="19"/>
       <c r="O12" s="8"/>
       <c r="P12" s="20"/>
@@ -1310,17 +1310,17 @@
     <row r="13" spans="1:16" ht="18" customHeight="1">
       <c r="A13" s="7"/>
       <c r="B13" s="9"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
       <c r="F13" s="14"/>
       <c r="G13" s="7"/>
       <c r="H13" s="15"/>
       <c r="I13" s="7"/>
       <c r="J13" s="21"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
       <c r="N13" s="14"/>
       <c r="O13" s="7"/>
       <c r="P13" s="15"/>
@@ -1328,17 +1328,17 @@
     <row r="14" spans="1:16" ht="18" customHeight="1">
       <c r="A14" s="8"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
       <c r="F14" s="19"/>
       <c r="G14" s="8"/>
       <c r="H14" s="20"/>
       <c r="I14" s="8"/>
       <c r="J14" s="22"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
       <c r="N14" s="19"/>
       <c r="O14" s="8"/>
       <c r="P14" s="20"/>
@@ -1346,17 +1346,17 @@
     <row r="15" spans="1:16" ht="18" customHeight="1">
       <c r="A15" s="7"/>
       <c r="B15" s="9"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
       <c r="F15" s="14"/>
       <c r="G15" s="7"/>
       <c r="H15" s="15"/>
       <c r="I15" s="7"/>
       <c r="J15" s="21"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
       <c r="N15" s="14"/>
       <c r="O15" s="7"/>
       <c r="P15" s="15"/>
@@ -1364,17 +1364,17 @@
     <row r="16" spans="1:16" ht="18" customHeight="1">
       <c r="A16" s="8"/>
       <c r="B16" s="10"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
       <c r="F16" s="19"/>
       <c r="G16" s="8"/>
       <c r="H16" s="20"/>
       <c r="I16" s="8"/>
       <c r="J16" s="22"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
       <c r="N16" s="19"/>
       <c r="O16" s="8"/>
       <c r="P16" s="20"/>
@@ -1382,17 +1382,17 @@
     <row r="17" spans="1:16" ht="18" customHeight="1">
       <c r="A17" s="7"/>
       <c r="B17" s="9"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
       <c r="F17" s="14"/>
       <c r="G17" s="7"/>
       <c r="H17" s="15"/>
       <c r="I17" s="7"/>
       <c r="J17" s="21"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
       <c r="N17" s="14"/>
       <c r="O17" s="7"/>
       <c r="P17" s="15"/>
@@ -1400,17 +1400,17 @@
     <row r="18" spans="1:16" ht="18" customHeight="1">
       <c r="A18" s="8"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
       <c r="F18" s="19"/>
       <c r="G18" s="8"/>
       <c r="H18" s="20"/>
       <c r="I18" s="8"/>
       <c r="J18" s="22"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
       <c r="N18" s="19"/>
       <c r="O18" s="8"/>
       <c r="P18" s="20"/>
@@ -1418,17 +1418,17 @@
     <row r="19" spans="1:16" ht="18" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
       <c r="F19" s="14"/>
       <c r="G19" s="7"/>
       <c r="H19" s="15"/>
       <c r="I19" s="7"/>
       <c r="J19" s="21"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
       <c r="N19" s="14"/>
       <c r="O19" s="7"/>
       <c r="P19" s="15"/>
@@ -1436,17 +1436,17 @@
     <row r="20" spans="1:16" ht="18" customHeight="1">
       <c r="A20" s="8"/>
       <c r="B20" s="10"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
       <c r="F20" s="19"/>
       <c r="G20" s="8"/>
       <c r="H20" s="20"/>
       <c r="I20" s="8"/>
       <c r="J20" s="22"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
       <c r="N20" s="19"/>
       <c r="O20" s="8"/>
       <c r="P20" s="20"/>
@@ -1454,17 +1454,17 @@
     <row r="21" spans="1:16" ht="18" customHeight="1">
       <c r="A21" s="7"/>
       <c r="B21" s="21"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
       <c r="F21" s="14"/>
       <c r="G21" s="7"/>
       <c r="H21" s="15"/>
       <c r="I21" s="7"/>
       <c r="J21" s="21"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
       <c r="N21" s="14"/>
       <c r="O21" s="7"/>
       <c r="P21" s="15"/>
@@ -1472,17 +1472,17 @@
     <row r="22" spans="1:16" ht="18" customHeight="1">
       <c r="A22" s="8"/>
       <c r="B22" s="22"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
       <c r="F22" s="19"/>
       <c r="G22" s="8"/>
       <c r="H22" s="20"/>
       <c r="I22" s="8"/>
       <c r="J22" s="22"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
       <c r="N22" s="19"/>
       <c r="O22" s="8"/>
       <c r="P22" s="20"/>
@@ -1490,17 +1490,17 @@
     <row r="23" spans="1:16" ht="18" customHeight="1">
       <c r="A23" s="7"/>
       <c r="B23" s="21"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
       <c r="F23" s="14"/>
       <c r="G23" s="7"/>
       <c r="H23" s="15"/>
       <c r="I23" s="7"/>
       <c r="J23" s="21"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="28"/>
       <c r="N23" s="14"/>
       <c r="O23" s="7"/>
       <c r="P23" s="15"/>
@@ -1508,17 +1508,17 @@
     <row r="24" spans="1:16" ht="18" customHeight="1">
       <c r="A24" s="8"/>
       <c r="B24" s="22"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
       <c r="F24" s="19"/>
       <c r="G24" s="8"/>
       <c r="H24" s="20"/>
       <c r="I24" s="8"/>
       <c r="J24" s="22"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
       <c r="N24" s="19"/>
       <c r="O24" s="8"/>
       <c r="P24" s="20"/>
@@ -1526,17 +1526,17 @@
     <row r="25" spans="1:16" ht="18" customHeight="1">
       <c r="A25" s="7"/>
       <c r="B25" s="9"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
       <c r="F25" s="14"/>
       <c r="G25" s="7"/>
       <c r="H25" s="15"/>
       <c r="I25" s="7"/>
       <c r="J25" s="21"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="28"/>
       <c r="N25" s="14"/>
       <c r="O25" s="7"/>
       <c r="P25" s="15"/>
@@ -1544,17 +1544,17 @@
     <row r="26" spans="1:16" ht="18" customHeight="1">
       <c r="A26" s="8"/>
       <c r="B26" s="10"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
       <c r="F26" s="19"/>
       <c r="G26" s="8"/>
       <c r="H26" s="20"/>
       <c r="I26" s="8"/>
       <c r="J26" s="22"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
       <c r="N26" s="19"/>
       <c r="O26" s="8"/>
       <c r="P26" s="20"/>
@@ -1562,17 +1562,17 @@
     <row r="27" spans="1:16" ht="19.5" customHeight="1">
       <c r="A27" s="7"/>
       <c r="B27" s="9"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
       <c r="F27" s="14"/>
       <c r="G27" s="7"/>
       <c r="H27" s="15"/>
       <c r="I27" s="7"/>
       <c r="J27" s="21"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="28"/>
       <c r="N27" s="14"/>
       <c r="O27" s="7"/>
       <c r="P27" s="15"/>
@@ -1580,17 +1580,17 @@
     <row r="28" spans="1:16" ht="18" customHeight="1">
       <c r="A28" s="8"/>
       <c r="B28" s="10"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
       <c r="F28" s="19"/>
       <c r="G28" s="8"/>
       <c r="H28" s="20"/>
       <c r="I28" s="8"/>
       <c r="J28" s="22"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
       <c r="N28" s="19"/>
       <c r="O28" s="8"/>
       <c r="P28" s="20"/>
@@ -1598,54 +1598,54 @@
     <row r="29" spans="1:16" ht="18.75" customHeight="1" thickBot="1">
       <c r="A29" s="7"/>
       <c r="B29" s="9"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
       <c r="F29" s="16"/>
       <c r="G29" s="17"/>
       <c r="H29" s="18"/>
       <c r="I29" s="7"/>
       <c r="J29" s="21"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
       <c r="N29" s="16"/>
       <c r="O29" s="17"/>
       <c r="P29" s="18"/>
     </row>
     <row r="30" spans="1:16" ht="27.75" customHeight="1">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="29"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="46"/>
+      <c r="N30" s="46"/>
     </row>
     <row r="31" spans="1:16" ht="24.75" customHeight="1">
-      <c r="A31" s="29"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="29"/>
+      <c r="A31" s="46"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
+      <c r="N31" s="46"/>
     </row>
     <row r="32" spans="1:16" ht="30" customHeight="1"/>
     <row r="33" ht="18" customHeight="1"/>
@@ -1671,39 +1671,19 @@
     <row r="54" ht="27.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="L4:N5"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
     <mergeCell ref="A30:N31"/>
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="C28:E28"/>
@@ -1717,26 +1697,46 @@
     <mergeCell ref="K29:M29"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="K24:M24"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="L4:N5"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:M11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="79" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="77" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <oddFooter>&amp;LDatasheets available for download at https://marinegeo.github.io/seagrass&amp;C&amp;"System Font,Regular"&amp;10&amp;K000000
 &amp;RPage __ of __</oddFooter>
-    <firstFooter>&amp;LDatasheets available for download at https://marinegeo.github.io/seagrass&amp;RPage __ of __</firstFooter>
+    <firstFooter>&amp;Lhttps://doi.org/10.25573/serc.14925114.v1</firstFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>